<commit_message>
Add bearings to BOM
</commit_message>
<xml_diff>
--- a/bom/bom.xlsx
+++ b/bom/bom.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Willem\Documents\Projecten\Balancing cube\bom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Willem\Documents\Projecten\Balancing cube\balancing-cube\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B66730-7543-48B3-8980-BA86CE9C2E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2AADDFF-057A-4B78-8C45-52A661766D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FA994236-878D-4C39-A221-8ACA43651A1B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="94">
   <si>
     <t>Name</t>
   </si>
@@ -301,6 +301,12 @@
   </si>
   <si>
     <t>Machine screw M3x8 countersunk (cornerstone - frame, frame - bridge)</t>
+  </si>
+  <si>
+    <t>Radial ball bearing, 4 mm x 9 mm x 4 mm (bore diameter x outer diameter x width)</t>
+  </si>
+  <si>
+    <t>638-4-ZZ-SKF</t>
   </si>
 </sst>
 </file>
@@ -664,7 +670,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35ACB939-A3C0-40BC-A0B8-1526923C6837}">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1158,7 +1164,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>4</v>
       </c>
@@ -1166,7 +1172,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>4</v>
       </c>
@@ -1174,7 +1180,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1</v>
       </c>
@@ -1182,7 +1188,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1</v>
       </c>
@@ -1190,7 +1196,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1</v>
       </c>
@@ -1198,7 +1204,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>9</v>
       </c>
@@ -1206,7 +1212,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>8</v>
       </c>
@@ -1214,7 +1220,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>8</v>
       </c>
@@ -1222,7 +1228,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>8</v>
       </c>
@@ -1230,7 +1236,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>9</v>
       </c>
@@ -1238,7 +1244,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>9</v>
       </c>
@@ -1246,12 +1252,23 @@
         <v>89</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>36</v>
       </c>
       <c r="B44" t="s">
         <v>91</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>3</v>
+      </c>
+      <c r="B45" t="s">
+        <v>92</v>
+      </c>
+      <c r="D45" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Organize esp32 <-> escon wiring
Remapped AO1 of M3 to an ADC1 pin.
Removed all three unused AO2 DI3 wirings and relevant diodes and capacitors
Corrected pins.h (Old version was not matching with old schematic btw)
Updated Bom accordingly
</commit_message>
<xml_diff>
--- a/bom/bom.xlsx
+++ b/bom/bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Willem\Documents\Projecten\Balancing cube\balancing-cube\bom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\balancing-cube2\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2AADDFF-057A-4B78-8C45-52A661766D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA5E7EA-05D5-4C63-8AEE-66A84A2668E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FA994236-878D-4C39-A221-8ACA43651A1B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{FA994236-878D-4C39-A221-8ACA43651A1B}"/>
   </bookViews>
   <sheets>
     <sheet name="bom" sheetId="1" r:id="rId1"/>
@@ -189,18 +189,12 @@
     <t>C12, C13</t>
   </si>
   <si>
-    <t>C6, C7, C8, C9, C10 C11, C14, C15, C16</t>
-  </si>
-  <si>
     <t>D1, D2, D3</t>
   </si>
   <si>
     <t>D4</t>
   </si>
   <si>
-    <t>D5, D6, D7, D8, D9, D10</t>
-  </si>
-  <si>
     <t>F1, F2, F3</t>
   </si>
   <si>
@@ -307,6 +301,12 @@
   </si>
   <si>
     <t>638-4-ZZ-SKF</t>
+  </si>
+  <si>
+    <t>C6, C7, C8, C9, C10, C11</t>
+  </si>
+  <si>
+    <t>D5, D6, D7</t>
   </si>
 </sst>
 </file>
@@ -358,7 +358,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -374,7 +374,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -672,18 +672,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35ACB939-A3C0-40BC-A0B8-1526923C6837}">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="80.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="35.42578125" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" customWidth="1"/>
+    <col min="2" max="2" width="80.81640625" customWidth="1"/>
+    <col min="3" max="3" width="36.6328125" customWidth="1"/>
+    <col min="4" max="4" width="35.453125" customWidth="1"/>
+    <col min="5" max="5" width="20.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -700,7 +702,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>3</v>
       </c>
@@ -714,10 +716,10 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -731,10 +733,10 @@
         <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1</v>
       </c>
@@ -748,27 +750,27 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2</v>
       </c>
@@ -782,10 +784,10 @@
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>3</v>
       </c>
@@ -793,16 +795,16 @@
         <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1</v>
       </c>
@@ -810,33 +812,33 @@
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
         <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>93</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>3</v>
       </c>
@@ -844,16 +846,16 @@
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D10" t="s">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>4</v>
       </c>
@@ -861,13 +863,13 @@
         <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>4</v>
       </c>
@@ -875,16 +877,16 @@
         <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>3</v>
       </c>
@@ -892,16 +894,16 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D13" t="s">
         <v>42</v>
       </c>
       <c r="E13" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>3</v>
       </c>
@@ -912,10 +914,10 @@
         <v>43</v>
       </c>
       <c r="E14" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1</v>
       </c>
@@ -923,16 +925,16 @@
         <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>1</v>
       </c>
@@ -940,16 +942,16 @@
         <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D16" t="s">
         <v>6</v>
       </c>
       <c r="E16" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2</v>
       </c>
@@ -957,16 +959,16 @@
         <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D17" t="s">
         <v>26</v>
       </c>
       <c r="E17" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>4</v>
       </c>
@@ -974,16 +976,16 @@
         <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D18" t="s">
         <v>28</v>
       </c>
       <c r="E18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>1</v>
       </c>
@@ -991,16 +993,16 @@
         <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D19" t="s">
         <v>30</v>
       </c>
       <c r="E19" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1008,16 +1010,16 @@
         <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D20" t="s">
         <v>32</v>
       </c>
       <c r="E20" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1025,16 +1027,16 @@
         <v>35</v>
       </c>
       <c r="C21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D21" t="s">
         <v>34</v>
       </c>
       <c r="E21" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1042,16 +1044,16 @@
         <v>37</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D22" t="s">
         <v>36</v>
       </c>
       <c r="E22" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>7</v>
       </c>
@@ -1062,10 +1064,10 @@
         <v>46</v>
       </c>
       <c r="E23" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>3</v>
       </c>
@@ -1076,10 +1078,10 @@
         <v>45</v>
       </c>
       <c r="E24" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1087,188 +1089,188 @@
         <v>39</v>
       </c>
       <c r="C25" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D25" t="s">
         <v>38</v>
       </c>
       <c r="E25" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D26" s="2">
         <v>591477</v>
       </c>
       <c r="E26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>3</v>
+      </c>
+      <c r="B27" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>3</v>
-      </c>
-      <c r="B27" t="s">
-        <v>74</v>
       </c>
       <c r="D27" s="2">
         <v>466023</v>
       </c>
       <c r="E27" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>9</v>
       </c>
       <c r="B38" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>8</v>
       </c>
       <c r="B41" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>9</v>
       </c>
       <c r="B43" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>36</v>
       </c>
       <c r="B44" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>3</v>
+      </c>
+      <c r="B45" t="s">
+        <v>90</v>
+      </c>
+      <c r="D45" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>3</v>
-      </c>
-      <c r="B45" t="s">
-        <v>92</v>
-      </c>
-      <c r="D45" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>